<commit_message>
merge 2 lvl grading
</commit_message>
<xml_diff>
--- a/data/GradingProtocol-2point.xlsx
+++ b/data/GradingProtocol-2point.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rizmehdi/Heriot-Watt University Team Dropbox/Mehdi Rizvi/UEA work/workshops/202512 Annotation Pilot Workshop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8CD9A65-7E6D-C542-B415-FEC8249209C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3013A99-E50B-8540-A4AE-060C23E8DE60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="500" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="protocol" sheetId="1" r:id="rId1"/>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>Understandability 3</t>
-  </si>
-  <si>
-    <t>Relevance </t>
   </si>
   <si>
     <t>The material is self-sufficeint and comprehensive and doesnt not require the reader to go to other documents or links for complete understanding of the policy </t>
@@ -167,6 +164,9 @@
   </si>
   <si>
     <t>Material doesnot specify Manageable, explicit steps or has no actions specified</t>
+  </si>
+  <si>
+    <t>Relevance</t>
   </si>
 </sst>
 </file>
@@ -504,8 +504,8 @@
   </sheetPr>
   <dimension ref="A1:R949"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -525,10 +525,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -547,16 +547,16 @@
     </row>
     <row r="2" spans="1:18" ht="42" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -578,13 +578,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -606,13 +606,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -634,13 +634,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -662,13 +662,13 @@
         <v>8</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -690,13 +690,13 @@
         <v>9</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -718,13 +718,13 @@
         <v>10</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -746,13 +746,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -774,13 +774,13 @@
         <v>6</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -802,13 +802,13 @@
         <v>7</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>

</xml_diff>